<commit_message>
shop progress then broke :(
updated elements to remove randoms
</commit_message>
<xml_diff>
--- a/resources/elements.xlsx
+++ b/resources/elements.xlsx
@@ -6,6 +6,7 @@
     <sheet state="visible" name="adjectives" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="nouns" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="of" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="enemies" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="286">
   <si>
     <t>name</t>
   </si>
@@ -246,15 +247,15 @@
     <t>king gizard, the</t>
   </si>
   <si>
+    <t>bass-boosted</t>
+  </si>
+  <si>
     <t>evil</t>
   </si>
   <si>
     <t>att</t>
   </si>
   <si>
-    <t>random</t>
-  </si>
-  <si>
     <t>def</t>
   </si>
   <si>
@@ -270,6 +271,9 @@
     <t>k</t>
   </si>
   <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>set</t>
   </si>
   <si>
@@ -717,9 +721,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>bad, abstract, wizard, machine, baseball, emotion, gun, throw, knight, classic, lgbt, cute, patriotic, gold, audio, basic, fancy</t>
   </si>
   <si>
@@ -739,6 +740,138 @@
   </si>
   <si>
     <t>cute, lgbt</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>charles</t>
+  </si>
+  <si>
+    <t>david</t>
+  </si>
+  <si>
+    <t>dylan</t>
+  </si>
+  <si>
+    <t>vinny</t>
+  </si>
+  <si>
+    <t>zach</t>
+  </si>
+  <si>
+    <t>glorbo</t>
+  </si>
+  <si>
+    <t>gorgug</t>
+  </si>
+  <si>
+    <t>grungo</t>
+  </si>
+  <si>
+    <t>bingus</t>
+  </si>
+  <si>
+    <t>bingy</t>
+  </si>
+  <si>
+    <t>bungo</t>
+  </si>
+  <si>
+    <t>greepy</t>
+  </si>
+  <si>
+    <t>flub</t>
+  </si>
+  <si>
+    <t>grub</t>
+  </si>
+  <si>
+    <t>gru</t>
+  </si>
+  <si>
+    <t>gub</t>
+  </si>
+  <si>
+    <t>grahm</t>
+  </si>
+  <si>
+    <t>griswaldo guthrie</t>
+  </si>
+  <si>
+    <t>gorshen grandiliquent</t>
+  </si>
+  <si>
+    <t>zig</t>
+  </si>
+  <si>
+    <t>zug</t>
+  </si>
+  <si>
+    <t>zog</t>
+  </si>
+  <si>
+    <t>bunkle</t>
+  </si>
+  <si>
+    <t>bunkis</t>
+  </si>
+  <si>
+    <t>nunkis</t>
+  </si>
+  <si>
+    <t>gumbo</t>
+  </si>
+  <si>
+    <t>zapdos</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>the strange</t>
+  </si>
+  <si>
+    <t>the elder</t>
+  </si>
+  <si>
+    <t>village idiot</t>
+  </si>
+  <si>
+    <t>the younger</t>
+  </si>
+  <si>
+    <t>the sleepy</t>
+  </si>
+  <si>
+    <t>&amp; bean</t>
+  </si>
+  <si>
+    <t>beepy, the eepy zeepy guy</t>
+  </si>
+  <si>
+    <t>greepus</t>
+  </si>
+  <si>
+    <t>bonkler</t>
+  </si>
+  <si>
+    <t>the shrew</t>
+  </si>
+  <si>
+    <t>spencer agnew</t>
+  </si>
+  <si>
+    <t>smith</t>
+  </si>
+  <si>
+    <t>the third</t>
+  </si>
+  <si>
+    <t>the fourth</t>
+  </si>
+  <si>
+    <t>the nineteen thousand, four hundred and fifty third</t>
   </si>
 </sst>
 </file>
@@ -817,6 +950,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1259,10 +1396,13 @@
       <c r="BZ1" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="CA1" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1">
         <v>0.0</v>
@@ -1399,8 +1539,8 @@
       <c r="AT2" s="1">
         <v>5.0</v>
       </c>
-      <c r="AU2" s="1" t="s">
-        <v>79</v>
+      <c r="AU2" s="1">
+        <v>0.0</v>
       </c>
       <c r="AV2" s="1">
         <v>9.0</v>
@@ -1493,6 +1633,9 @@
         <v>9.0</v>
       </c>
       <c r="BZ2" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="CA2" s="1">
         <v>6.0</v>
       </c>
     </row>
@@ -1635,8 +1778,8 @@
       <c r="AT3" s="1">
         <v>6.0</v>
       </c>
-      <c r="AU3" s="1" t="s">
-        <v>79</v>
+      <c r="AU3" s="1">
+        <v>0.0</v>
       </c>
       <c r="AV3" s="1">
         <v>0.0</v>
@@ -1729,6 +1872,9 @@
         <v>9.0</v>
       </c>
       <c r="BZ3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="CA3" s="1">
         <v>3.0</v>
       </c>
     </row>
@@ -1868,11 +2014,11 @@
       <c r="AS4" s="1">
         <v>0.0</v>
       </c>
-      <c r="AT4" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AU4" s="1" t="s">
-        <v>79</v>
+      <c r="AT4" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="AU4" s="1">
+        <v>0.0</v>
       </c>
       <c r="AV4" s="1">
         <v>9.0</v>
@@ -1965,6 +2111,9 @@
         <v>9.0</v>
       </c>
       <c r="BZ4" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="CA4" s="1">
         <v>6.0</v>
       </c>
     </row>
@@ -2274,98 +2423,101 @@
       <c r="BY5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BZ5" s="1" t="str">
-        <f>LEFT(BZ1)</f>
+      <c r="BZ5" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CA5" s="1" t="str">
+        <f>LEFT(CA1)</f>
         <v>e</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="M6" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Y6" s="1" t="s">
         <v>47</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AD6" s="1" t="s">
         <v>30</v>
@@ -2377,147 +2529,150 @@
         <v>30</v>
       </c>
       <c r="AG6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AI6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AO6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AH6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AJ6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AK6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AL6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AM6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AN6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AO6" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="AP6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AQ6" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AR6" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="AS6" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AT6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AU6" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AV6" s="1" t="s">
         <v>47</v>
       </c>
       <c r="AW6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AX6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AY6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AZ6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BB6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BC6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BD6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BE6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BF6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BG6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BH6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BI6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="BJ6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="BK6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BL6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BM6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BN6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="BO6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BP6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BQ6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="BR6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BS6" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="AY6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AZ6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BA6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="BB6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BC6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BD6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BE6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="BF6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BG6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BH6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BI6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="BJ6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="BK6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BL6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="BM6" s="1" t="s">
+      <c r="BT6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BU6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BV6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BW6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BX6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BY6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="BZ6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="BN6" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BO6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="BP6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BQ6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="BR6" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="BS6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="BT6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="BU6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="BV6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BW6" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BX6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="BY6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="BZ6" s="1" t="s">
-        <v>105</v>
+      <c r="CA6" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B7" s="1">
         <v>16.0</v>
@@ -2748,6 +2903,9 @@
         <v>2.0</v>
       </c>
       <c r="BZ7" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="CA7" s="1">
         <v>9.0</v>
       </c>
     </row>
@@ -2774,198 +2932,198 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I1" s="1">
         <v>9.0</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="BG1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="BH1" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="BI1" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="BJ1" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="BK1" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="BL1" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="BM1" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" ht="21.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1">
         <v>0.0</v>
@@ -3090,8 +3248,8 @@
       <c r="AP2" s="1">
         <v>10.0</v>
       </c>
-      <c r="AQ2" s="1" t="s">
-        <v>79</v>
+      <c r="AQ2" s="1">
+        <v>0.0</v>
       </c>
       <c r="AR2" s="1">
         <v>-5.0</v>
@@ -3287,8 +3445,8 @@
       <c r="AP3" s="1">
         <v>3.0</v>
       </c>
-      <c r="AQ3" s="1" t="s">
-        <v>79</v>
+      <c r="AQ3" s="1">
+        <v>0.0</v>
       </c>
       <c r="AR3" s="1">
         <v>0.0</v>
@@ -3484,8 +3642,8 @@
       <c r="AP4" s="1">
         <v>2.0</v>
       </c>
-      <c r="AQ4" s="1" t="s">
-        <v>79</v>
+      <c r="AQ4" s="1">
+        <v>0.0</v>
       </c>
       <c r="AR4" s="1">
         <v>-10.0</v>
@@ -3715,7 +3873,7 @@
         <v>a</v>
       </c>
       <c r="AO5" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="AP5" s="1" t="str">
         <f t="shared" ref="AP5:BM5" si="2">LEFT(AP1)</f>
@@ -3816,204 +3974,204 @@
     </row>
     <row r="6" ht="21.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="N6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="S6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y6" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="Z6" s="1" t="s">
         <v>47</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AJ6" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AM6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AO6" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AP6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AQ6" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AR6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="AS6" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AT6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AU6" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AV6" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AW6" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AY6" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AZ6" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="BA6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="BB6" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BC6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="BD6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="BE6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="BF6" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="BG6" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="BH6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="BI6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="BJ6" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="BK6" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BL6" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BM6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B7" s="1">
         <v>16.0</v>
@@ -4231,138 +4389,138 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1">
         <v>0.0</v>
@@ -4421,8 +4579,8 @@
       <c r="T2" s="1">
         <v>2.0</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>79</v>
+      <c r="U2" s="1">
+        <v>0.0</v>
       </c>
       <c r="V2" s="1">
         <v>3.0</v>
@@ -4558,8 +4716,8 @@
       <c r="T3" s="1">
         <v>0.0</v>
       </c>
-      <c r="U3" s="1" t="s">
-        <v>79</v>
+      <c r="U3" s="1">
+        <v>0.0</v>
       </c>
       <c r="V3" s="1">
         <v>10.0</v>
@@ -4695,8 +4853,8 @@
       <c r="T4" s="1">
         <v>13.0</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>79</v>
+      <c r="U4" s="1">
+        <v>0.0</v>
       </c>
       <c r="V4" s="1">
         <v>2.0</v>
@@ -4832,10 +4990,10 @@
         <v>b</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="R5" s="4" t="str">
         <f t="shared" ref="R5:S5" si="2">MID(R1,4,1)</f>
@@ -4846,10 +5004,10 @@
         <v>s</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="V5" s="4" t="str">
         <f t="shared" ref="V5:W5" si="3">MID(V1,4,1)</f>
@@ -4860,27 +5018,27 @@
         <v>s</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AA5" s="4" t="str">
         <f>MID(AA1,4,1)</f>
         <v>t</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AC5" s="4" t="str">
         <f>MID(AC1,4,1)</f>
         <v>p</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AE5" s="4" t="str">
         <f t="shared" ref="AE5:AI5" si="4">MID(AE1,4,1)</f>
@@ -4903,16 +5061,16 @@
         <v>s</v>
       </c>
       <c r="AJ5" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AK5" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AL5" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="AN5" s="4" t="str">
         <f t="shared" ref="AN5:AP5" si="5">MID(AN1,4,1)</f>
@@ -4927,7 +5085,7 @@
         <v>c</v>
       </c>
       <c r="AQ5" s="1" t="s">
-        <v>234</v>
+        <v>85</v>
       </c>
       <c r="AR5" s="4" t="str">
         <f t="shared" ref="AR5:AS5" si="6">MID(AR1,4,1)</f>
@@ -4940,25 +5098,25 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>235</v>
@@ -4967,22 +5125,22 @@
         <v>47</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>30</v>
@@ -4991,64 +5149,64 @@
         <v>30</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>236</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="AB6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AG6" s="1" t="s">
         <v>237</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AI6" s="1" t="s">
         <v>238</v>
       </c>
       <c r="AJ6" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AL6" s="1" t="s">
         <v>239</v>
@@ -5057,19 +5215,19 @@
         <v>240</v>
       </c>
       <c r="AN6" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="AO6" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AP6" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="AQ6" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AR6" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AS6" s="1" t="s">
         <v>241</v>
@@ -5077,7 +5235,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B7" s="1">
         <v>50.0</v>
@@ -5278,4 +5436,155 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>